<commit_message>
adding calibration data and hitch controller
</commit_message>
<xml_diff>
--- a/calibration_sheet.xlsx
+++ b/calibration_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JeremyNoonan\Documents\github\massey_3545_hitch_controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FDFB716-3AC2-435B-A1A2-2C0F37A89AEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D152410F-8917-4DEC-981A-C66E3DAEE5C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17023" yWindow="0" windowWidth="15891" windowHeight="20571" xr2:uid="{0D881AED-880D-4F73-AA28-7B0266F46ED7}"/>
   </bookViews>
@@ -33,6 +33,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -395,8 +417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F389ED4-3E5B-4518-8BA6-57C13E54178F}">
   <dimension ref="A1:C157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="C146" sqref="C146"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="C122" sqref="C122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -405,7 +427,7 @@
     <col min="2" max="2" width="16.765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -413,15 +435,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>120</v>
       </c>
       <c r="B2">
         <v>301</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C2" cm="1">
+        <f t="array" aca="1" ref="C2" ca="1">_xlfn.UNIQUE(B2:C107157)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>119</v>
       </c>
@@ -429,7 +455,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>118</v>
       </c>
@@ -437,7 +463,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>117</v>
       </c>
@@ -445,7 +471,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>116</v>
       </c>
@@ -453,7 +479,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>115</v>
       </c>
@@ -461,7 +487,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>114</v>
       </c>
@@ -469,7 +495,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>113</v>
       </c>
@@ -477,7 +503,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>112</v>
       </c>
@@ -485,7 +511,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>111</v>
       </c>
@@ -493,7 +519,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>110</v>
       </c>
@@ -501,7 +527,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>109</v>
       </c>
@@ -509,7 +535,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>108</v>
       </c>
@@ -517,7 +543,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>107</v>
       </c>
@@ -525,7 +551,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>106</v>
       </c>
@@ -1173,7 +1199,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A97">
         <v>25</v>
       </c>
@@ -1181,7 +1207,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A98">
         <v>24</v>
       </c>
@@ -1189,7 +1215,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A99">
         <v>23</v>
       </c>
@@ -1197,7 +1223,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A100">
         <v>22</v>
       </c>
@@ -1205,7 +1231,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A101">
         <v>21</v>
       </c>
@@ -1213,7 +1239,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A102">
         <v>20</v>
       </c>
@@ -1221,7 +1247,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A103">
         <v>19</v>
       </c>
@@ -1229,7 +1255,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A104">
         <v>18</v>
       </c>
@@ -1237,7 +1263,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A105">
         <v>17</v>
       </c>
@@ -1245,7 +1271,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A106">
         <v>16</v>
       </c>
@@ -1253,18 +1279,15 @@
         <v>409</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A107">
         <v>15</v>
       </c>
       <c r="B107">
         <v>409</v>
       </c>
-      <c r="C107">
-        <v>-409</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.4">
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A108">
         <v>14</v>
       </c>
@@ -1272,7 +1295,7 @@
         <v>-409</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A109">
         <v>13</v>
       </c>
@@ -1280,7 +1303,7 @@
         <v>-408</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A110">
         <v>12</v>
       </c>
@@ -1288,7 +1311,7 @@
         <v>-407</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A111">
         <v>11</v>
       </c>
@@ -1296,7 +1319,7 @@
         <v>-407</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A112">
         <v>10</v>
       </c>

</xml_diff>